<commit_message>
big changes done to mask images (23.04.2024)
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SANCHDI2\OneDrive - Alcon\Desktop\Blasenentfernung\dioptre_reduzierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SANCHDI2\OneDrive - Alcon\GitHub\dioptre_reduzierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC96B29-E557-4465-8D9C-E14C95A6AF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D00E96-75AE-4FC9-BB7C-D99DE58976F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -546,7 +557,7 @@
   <dimension ref="A1:D415"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>